<commit_message>
Now array fields don't need []
</commit_message>
<xml_diff>
--- a/Assets/ExcelToClassParser/Demo/Excel/TestSheet.xlsx
+++ b/Assets/ExcelToClassParser/Demo/Excel/TestSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -46,10 +46,10 @@
     <t xml:space="preserve">Intellect</t>
   </si>
   <si>
-    <t xml:space="preserve">PastTimes[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skills[]</t>
+    <t xml:space="preserve">PastTimes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skills</t>
   </si>
   <si>
     <t xml:space="preserve">Image</t>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">Goblin</t>
   </si>
   <si>
+    <t xml:space="preserve">1.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">building,수리하기,ひらがな</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
+    <t xml:space="preserve">2.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">drinkin,eatin,fightin,sleepin</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
+    <t xml:space="preserve">12.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file02</t>
   </si>
   <si>
@@ -112,6 +121,9 @@
     <t xml:space="preserve">6</t>
   </si>
   <si>
+    <t xml:space="preserve">15.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file03</t>
   </si>
   <si>
@@ -121,6 +133,9 @@
     <t xml:space="preserve">7</t>
   </si>
   <si>
+    <t xml:space="preserve">3.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file04</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
     <t xml:space="preserve">8</t>
   </si>
   <si>
+    <t xml:space="preserve">6.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file05</t>
   </si>
   <si>
@@ -139,6 +157,9 @@
     <t xml:space="preserve">9</t>
   </si>
   <si>
+    <t xml:space="preserve">4.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file06</t>
   </si>
   <si>
@@ -148,6 +169,9 @@
     <t xml:space="preserve">10</t>
   </si>
   <si>
+    <t xml:space="preserve">7.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file07</t>
   </si>
   <si>
@@ -157,6 +181,9 @@
     <t xml:space="preserve">11</t>
   </si>
   <si>
+    <t xml:space="preserve">4.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file08</t>
   </si>
   <si>
@@ -166,6 +193,9 @@
     <t xml:space="preserve">12</t>
   </si>
   <si>
+    <t xml:space="preserve">9.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file09</t>
   </si>
   <si>
@@ -175,6 +205,9 @@
     <t xml:space="preserve">41</t>
   </si>
   <si>
+    <t xml:space="preserve">8.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file10</t>
   </si>
   <si>
@@ -184,6 +217,9 @@
     <t xml:space="preserve">35</t>
   </si>
   <si>
+    <t xml:space="preserve">4.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reources/file11</t>
   </si>
   <si>
@@ -191,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3</t>
   </si>
   <si>
     <t xml:space="preserve">Reources/file12</t>
@@ -331,7 +370,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,95 +436,95 @@
       <c r="F2" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="n">
-        <v>5</v>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G3" s="3" t="n">
-        <v>11</v>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="G4" s="3" t="n">
-        <v>100</v>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>100</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -497,100 +536,100 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="n">
-        <v>5</v>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G6" s="3" t="n">
-        <v>11</v>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>15</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>100</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="G7" s="3" t="n">
-        <v>100</v>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>100</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>12</v>
@@ -602,100 +641,100 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G8" s="3" t="n">
-        <v>5</v>
+      <c r="G8" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G9" s="3" t="n">
-        <v>11</v>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>15</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>100</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="G10" s="3" t="n">
-        <v>100</v>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>100</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -707,100 +746,100 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G11" s="3" t="n">
-        <v>5</v>
+      <c r="G11" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G12" s="3" t="n">
-        <v>11</v>
+      <c r="G12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>15</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>100</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="G13" s="3" t="n">
-        <v>100</v>
+      <c r="G13" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>100</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
@@ -812,25 +851,25 @@
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G14" s="3" t="n">
-        <v>5</v>
+      <c r="G14" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>